<commit_message>
mm 5 6 7 8 for me and ches
</commit_message>
<xml_diff>
--- a/mm/Алимбеков дкип-481 лр5.xlsx
+++ b/mm/Алимбеков дкип-481 лр5.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Labs\mm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erzat\Desktop\Labs\mm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C121A6D-1D61-45C3-8071-42C326CEC7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D955A73B-3207-4B78-9083-7782AD5A1BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="4" r:id="rId2"/>
+    <sheet name="Лист2" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Лист1!$B$4:$C$4</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Лист2!$B$6:$C$6</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
@@ -29,17 +30,17 @@
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Лист1!$B$4</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Лист2!$B$6</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Лист2!$D$3</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Лист1!$C$4</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Лист2!$C$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Лист2!$D$4</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Лист1!$D$2</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Лист2!$D$3</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Лист2!$D$5</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Лист1!$D$3</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Лист2!$D$4</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Лист2!$D$5</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
@@ -48,37 +49,35 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Лист1!$M$8</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Лист1!$B$6</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Лист2!$B$8</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">Лист2!$E$3</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Лист2!$E$4</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Лист1!$E$2</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Лист2!$E$3</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Лист2!$E$5</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">Лист1!$E$3</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Лист2!$E$4</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Лист2!$E$5</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">0</definedName>
@@ -106,8 +105,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -115,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>X1</t>
   </si>
@@ -144,9 +141,6 @@
     <t>прибыль</t>
   </si>
   <si>
-    <t>общая прибыль</t>
-  </si>
-  <si>
     <t>затраты рес</t>
   </si>
   <si>
@@ -156,7 +150,16 @@
     <t>количество</t>
   </si>
   <si>
-    <t>371, 4</t>
+    <t xml:space="preserve">шкафы - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">столы - </t>
+  </si>
+  <si>
+    <t>x1 =</t>
+  </si>
+  <si>
+    <t>x2 =</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +194,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -228,11 +237,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -246,13 +325,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -270,6 +367,114 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>17584</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>17584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>583349</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>157089</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64ED7E3D-9D39-4489-AE3D-9DD55767650D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3675184" y="199292"/>
+          <a:ext cx="3613765" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>69607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC848A46-7D60-9910-780F-AFB75153BCDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4351020" y="198121"/>
+          <a:ext cx="4381500" cy="1883166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,15 +740,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -554,7 +759,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -565,14 +770,14 @@
         <v>3</v>
       </c>
       <c r="D2" s="1">
-        <f>B2+3*C2</f>
-        <v>10</v>
+        <f>B2*B4+C4*C2</f>
+        <v>9</v>
       </c>
       <c r="E2" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -583,25 +788,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <f>B3+C3</f>
-        <v>2</v>
+        <f>B3*B4+C3*C4</f>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -612,39 +817,56 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <f>B5*B4+C5*C4</f>
-        <v>5</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA2D9D1-DC16-49AA-99B2-B777225487D3}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B04BF5-6590-4745-BF17-1D0C24942DCD}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -652,101 +874,161 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>0.2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>0.1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <f>B3*B6+C3*C6</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="E3" s="8">
+        <v>37.000000102463218</v>
+      </c>
+      <c r="E3" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="9">
         <v>0.1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>0.3</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <f>B4*B6+C4*C6</f>
-        <v>0.4</v>
-      </c>
-      <c r="E4" s="8">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <v>1.2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>1.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <f>B5*B6+C5*C6</f>
-        <v>2.7</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>371.40000043034553</v>
+      </c>
+      <c r="E5" s="7">
+        <v>371.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11">
+        <v>102.00000061477932</v>
+      </c>
+      <c r="C6" s="11">
+        <v>165.99999979507356</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <f>B7*B6+C7*C6</f>
-        <v>14</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B8" s="9">
+        <f>B6*B7+C6*C7</f>
+        <v>1940.0000020492644</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="12">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="16">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>